<commit_message>
Reading Excel to Two-dim
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/hrm_data.xlsx
+++ b/src/test/resources/test_data/hrm_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Session\automation_workspace\HealthManagmentAutomation\src\test\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -43,9 +43,6 @@
     <t>saul</t>
   </si>
   <si>
-    <t>saul1223</t>
-  </si>
-  <si>
     <t>Invalid credentials</t>
   </si>
   <si>
@@ -53,6 +50,12 @@
   </si>
   <si>
     <t>kim123</t>
+  </si>
+  <si>
+    <t>bala</t>
+  </si>
+  <si>
+    <t>bala123</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,22 +413,33 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>123344</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>